<commit_message>
Interface created, todo's and more firms
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Reports.xlsx
+++ b/src/main/resources/baseFiles/excel/Reports.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="37">
   <si>
     <t>Firm</t>
   </si>
@@ -63,6 +63,108 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>Appleby Global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09s
+</t>
+  </si>
+  <si>
+    <t>Aron Tadmor Levy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15s
+</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Anand And Anand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05s
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06s
+</t>
+  </si>
+  <si>
+    <t>ALMTLegal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14s
+</t>
+  </si>
+  <si>
+    <t>Ashurst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10s
+</t>
+  </si>
+  <si>
+    <t>Arnold And Porter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18s
+</t>
+  </si>
+  <si>
+    <t>Bae Kim And Lee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59s
+</t>
+  </si>
+  <si>
+    <t>Al Tamimi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24s
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08s
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04s
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03s
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01min 00s
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23s
+</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21s
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04min 03s
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03min 02s
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51s
+</t>
   </si>
 </sst>
 </file>
@@ -468,7 +570,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A350BCBC-CDDB-414C-9A72-BE6A09964F3F}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -493,24 +595,79 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>8</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2nd time using, small fixes
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Reports.xlsx
+++ b/src/main/resources/baseFiles/excel/Reports.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="103">
   <si>
     <t>Firm</t>
   </si>
@@ -264,6 +264,105 @@
   </si>
   <si>
     <t>Dahl Law</t>
+  </si>
+  <si>
+    <t>Havel Partners</t>
+  </si>
+  <si>
+    <t>17s</t>
+  </si>
+  <si>
+    <t>Blakes</t>
+  </si>
+  <si>
+    <t>51s</t>
+  </si>
+  <si>
+    <t>Mijares Angoitia Cortés And Fuentes</t>
+  </si>
+  <si>
+    <t>07s</t>
+  </si>
+  <si>
+    <t>Hill Dickinson</t>
+  </si>
+  <si>
+    <t>McCarthy Tetrault</t>
+  </si>
+  <si>
+    <t>Bennett Jones</t>
+  </si>
+  <si>
+    <t>18s</t>
+  </si>
+  <si>
+    <t>Howse Williams</t>
+  </si>
+  <si>
+    <t>Jones Day</t>
+  </si>
+  <si>
+    <t>Cassels</t>
+  </si>
+  <si>
+    <t>01min 05s</t>
+  </si>
+  <si>
+    <t>Ritch Mueller And Nicolau</t>
+  </si>
+  <si>
+    <t>Krogerus</t>
+  </si>
+  <si>
+    <t>Latham And Watkins</t>
+  </si>
+  <si>
+    <t>20s</t>
+  </si>
+  <si>
+    <t>Kinstellar</t>
+  </si>
+  <si>
+    <t>42s</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Lee And Ko</t>
+  </si>
+  <si>
+    <t>19s</t>
+  </si>
+  <si>
+    <t>Stikeman Elliott</t>
+  </si>
+  <si>
+    <t>01min 19s</t>
+  </si>
+  <si>
+    <t>Hannes Snellman</t>
+  </si>
+  <si>
+    <t>Peter And Kim</t>
+  </si>
+  <si>
+    <t>Kromann Reumert</t>
+  </si>
+  <si>
+    <t>Hakun Law</t>
+  </si>
+  <si>
+    <t>Greenberg Traurig</t>
+  </si>
+  <si>
+    <t>HFW</t>
+  </si>
+  <si>
+    <t>03min 47s</t>
+  </si>
+  <si>
+    <t>BLG Law</t>
   </si>
 </sst>
 </file>
@@ -669,7 +768,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A350BCBC-CDDB-414C-9A72-BE6A09964F3F}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -694,21 +793,21 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s" s="2">
         <v>13</v>
@@ -716,43 +815,43 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s" s="2">
         <v>42</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s" s="2">
         <v>40</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s" s="2">
         <v>13</v>
@@ -760,32 +859,32 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s" s="2">
         <v>13</v>
@@ -793,10 +892,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s" s="2">
         <v>13</v>
@@ -804,84 +903,84 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>13</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s" s="2">
         <v>47</v>
@@ -892,78 +991,56 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="B25" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="C25" t="s" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="B26" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="C26" t="s" s="2">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
3rd time using it
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Reports.xlsx
+++ b/src/main/resources/baseFiles/excel/Reports.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="147">
   <si>
     <t>Firm</t>
   </si>
@@ -363,6 +363,138 @@
   </si>
   <si>
     <t>BLG Law</t>
+  </si>
+  <si>
+    <t>Schoenherr</t>
+  </si>
+  <si>
+    <t>Cassidy Levy Kent</t>
+  </si>
+  <si>
+    <t>44s</t>
+  </si>
+  <si>
+    <t>Magnusson Law</t>
+  </si>
+  <si>
+    <t>Reliance Corporate Advisors</t>
+  </si>
+  <si>
+    <t>Fox And Mandal</t>
+  </si>
+  <si>
+    <t>Spruson And Ferguson</t>
+  </si>
+  <si>
+    <t>35s</t>
+  </si>
+  <si>
+    <t>Winston And Strawn</t>
+  </si>
+  <si>
+    <t>White And Case</t>
+  </si>
+  <si>
+    <t>02min 56s</t>
+  </si>
+  <si>
+    <t>Walkers</t>
+  </si>
+  <si>
+    <t>25s</t>
+  </si>
+  <si>
+    <t>McMillan</t>
+  </si>
+  <si>
+    <t>06min 52s</t>
+  </si>
+  <si>
+    <t>Meitar Law</t>
+  </si>
+  <si>
+    <t>Tiruchelvam Associates</t>
+  </si>
+  <si>
+    <t>Crowell And Moring</t>
+  </si>
+  <si>
+    <t>31s</t>
+  </si>
+  <si>
+    <t>Tuca Zbarcea</t>
+  </si>
+  <si>
+    <t>MZM Legal</t>
+  </si>
+  <si>
+    <t>Titov</t>
+  </si>
+  <si>
+    <t>Taylor Wessing</t>
+  </si>
+  <si>
+    <t>Ropes And Gray</t>
+  </si>
+  <si>
+    <t>Pedersoli</t>
+  </si>
+  <si>
+    <t>01min 04s</t>
+  </si>
+  <si>
+    <t>LEX Logmannsstofa</t>
+  </si>
+  <si>
+    <t>Finreg 360</t>
+  </si>
+  <si>
+    <t>ShinAndKim</t>
+  </si>
+  <si>
+    <t>NPP Legal</t>
+  </si>
+  <si>
+    <t>Spencer West</t>
+  </si>
+  <si>
+    <t>26s</t>
+  </si>
+  <si>
+    <t>Watson Farley And Williams</t>
+  </si>
+  <si>
+    <t>33s</t>
+  </si>
+  <si>
+    <t>Panetta Consulting Group</t>
+  </si>
+  <si>
+    <t>Njord</t>
+  </si>
+  <si>
+    <t>06min 17s</t>
+  </si>
+  <si>
+    <t>VB Advocates</t>
+  </si>
+  <si>
+    <t>SEUM</t>
+  </si>
+  <si>
+    <t>23s</t>
+  </si>
+  <si>
+    <t>Malley And Co</t>
+  </si>
+  <si>
+    <t>02s</t>
+  </si>
+  <si>
+    <t>Matheson</t>
+  </si>
+  <si>
+    <t>Wolf Theiss</t>
   </si>
 </sst>
 </file>
@@ -768,7 +900,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A350BCBC-CDDB-414C-9A72-BE6A09964F3F}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -793,87 +925,87 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s" s="2">
         <v>5</v>
@@ -881,32 +1013,32 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s" s="2">
         <v>13</v>
@@ -914,43 +1046,43 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>90</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s" s="2">
         <v>32</v>
@@ -958,10 +1090,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s" s="2">
         <v>13</v>
@@ -969,21 +1101,21 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s" s="2">
         <v>13</v>
@@ -991,57 +1123,200 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s" s="2">
         <v>13</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="B25" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="B26" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="B27" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="C27" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="B28" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="C28" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="C29" t="s" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="B30" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="C30" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="B31" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="B32" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="C32" t="s" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="B33" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="C33" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="B34" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="C34" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="B35" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="C35" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="B36" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="B37" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="C37" t="s" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4th time using it. Improve OFFICE_CHECK in the SiteUtls
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Reports.xlsx
+++ b/src/main/resources/baseFiles/excel/Reports.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="180">
   <si>
     <t>Firm</t>
   </si>
@@ -540,6 +540,60 @@
   </si>
   <si>
     <t>Minter Ellison RuddWatts</t>
+  </si>
+  <si>
+    <t>SFKS Law</t>
+  </si>
+  <si>
+    <t>41s</t>
+  </si>
+  <si>
+    <t>AWA</t>
+  </si>
+  <si>
+    <t>VO Patents And Trademarks</t>
+  </si>
+  <si>
+    <t>34s</t>
+  </si>
+  <si>
+    <t>Tavares</t>
+  </si>
+  <si>
+    <t>LEFOSSE</t>
+  </si>
+  <si>
+    <t>DaleAndLessmann</t>
+  </si>
+  <si>
+    <t>MBIP</t>
+  </si>
+  <si>
+    <t>Kolster</t>
+  </si>
+  <si>
+    <t>37s</t>
+  </si>
+  <si>
+    <t>BARDEHLE PAGENBERG</t>
+  </si>
+  <si>
+    <t>Viering Jentschura And Partner</t>
+  </si>
+  <si>
+    <t>Hammarskiöld And Co</t>
+  </si>
+  <si>
+    <t>01min 09s</t>
+  </si>
+  <si>
+    <t>01min 13s</t>
+  </si>
+  <si>
+    <t>Drzewiecki Tomaszek</t>
+  </si>
+  <si>
+    <t>Aguayo Ecclefield And Martinez</t>
   </si>
 </sst>
 </file>
@@ -945,7 +999,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A350BCBC-CDDB-414C-9A72-BE6A09964F3F}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -970,7 +1024,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>127</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s" s="2">
         <v>61</v>
@@ -981,10 +1035,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>147</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>148</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s" s="2">
         <v>13</v>
@@ -992,21 +1046,21 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>149</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>150</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s" s="2">
         <v>13</v>
@@ -1014,87 +1068,87 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>153</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>64</v>
+        <v>138</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>156</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>63</v>
+        <v>148</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>104</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>142</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s" s="2">
         <v>54</v>
@@ -1102,43 +1156,43 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>46</v>
+        <v>166</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>159</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s" s="2">
         <v>13</v>
@@ -1146,24 +1200,376 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>106</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>121</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="B19" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="B20" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="B22" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="C22" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="B24" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="B26" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="C27" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="C28" t="s" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="C29" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="B30" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="B31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="2">
         <v>161</v>
       </c>
-      <c r="B19" t="s" s="2">
+      <c r="B32" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="B34" t="s" s="2">
         <v>56</v>
       </c>
-      <c r="C19" t="s" s="2">
-        <v>13</v>
+      <c r="C34" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="B35" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="C35" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="C36" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="C37" t="s" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="B38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="C38" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="B39" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="C39" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="B40" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="B41" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C41" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="B42" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="C42" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="B43" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="C43" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="B44" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="C44" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="B46" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="C46" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="C47" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="B48" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="C48" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="C49" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="B51" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="C51" t="s" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete the Contacts Already Registered class. Completely working. Improve the classes of Excel, minor changes of lawyers class, fixes in the sites children. 5th time using
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Reports.xlsx
+++ b/src/main/resources/baseFiles/excel/Reports.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="213">
   <si>
     <t>Firm</t>
   </si>
@@ -594,6 +594,105 @@
   </si>
   <si>
     <t>Aguayo Ecclefield And Martinez</t>
+  </si>
+  <si>
+    <t>AL Goodbody</t>
+  </si>
+  <si>
+    <t>40s</t>
+  </si>
+  <si>
+    <t>Dottir</t>
+  </si>
+  <si>
+    <t>Frontier</t>
+  </si>
+  <si>
+    <t>03min 26s</t>
+  </si>
+  <si>
+    <t>15s</t>
+  </si>
+  <si>
+    <t>DR And AJU</t>
+  </si>
+  <si>
+    <t>BCF Law</t>
+  </si>
+  <si>
+    <t>MSP</t>
+  </si>
+  <si>
+    <t>Nelligan Law</t>
+  </si>
+  <si>
+    <t>Beauchamps</t>
+  </si>
+  <si>
+    <t>49s</t>
+  </si>
+  <si>
+    <t>Tompkins Wake</t>
+  </si>
+  <si>
+    <t>Andersen</t>
+  </si>
+  <si>
+    <t>Arnesen IP</t>
+  </si>
+  <si>
+    <t>Oyen Wiggs</t>
+  </si>
+  <si>
+    <t>DCC Law</t>
+  </si>
+  <si>
+    <t>39s</t>
+  </si>
+  <si>
+    <t>Zamfirescu Racoti Predoiu</t>
+  </si>
+  <si>
+    <t>Stephenson Harwood</t>
+  </si>
+  <si>
+    <t>StewartMcKelvey</t>
+  </si>
+  <si>
+    <t>DBHLaw</t>
+  </si>
+  <si>
+    <t>Liedekerke</t>
+  </si>
+  <si>
+    <t>38s</t>
+  </si>
+  <si>
+    <t>24s</t>
+  </si>
+  <si>
+    <t>Barriston Law</t>
+  </si>
+  <si>
+    <t>Borenius</t>
+  </si>
+  <si>
+    <t>Ogletree Deakins</t>
+  </si>
+  <si>
+    <t>James And Wells</t>
+  </si>
+  <si>
+    <t>Brigrard Urrutia</t>
+  </si>
+  <si>
+    <t>Covenant Chambers</t>
+  </si>
+  <si>
+    <t>Barnea And Co</t>
+  </si>
+  <si>
+    <t>27s</t>
   </si>
 </sst>
 </file>
@@ -999,7 +1098,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A350BCBC-CDDB-414C-9A72-BE6A09964F3F}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -1024,32 +1123,32 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>61</v>
+        <v>181</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>80</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s" s="2">
         <v>13</v>
@@ -1057,32 +1156,32 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>84</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>68</v>
+        <v>183</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>141</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s" s="2">
         <v>13</v>
@@ -1090,76 +1189,76 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>138</v>
+        <v>186</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>130</v>
+        <v>188</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>125</v>
+        <v>189</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>40</v>
+        <v>191</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>123</v>
+        <v>192</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s" s="2">
         <v>13</v>
@@ -1167,43 +1266,43 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>155</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>166</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>167</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>46</v>
+        <v>172</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s" s="2">
         <v>13</v>
@@ -1211,21 +1310,21 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>169</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>47</v>
+        <v>177</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s" s="2">
         <v>13</v>
@@ -1233,40 +1332,40 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>74</v>
+        <v>194</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>40</v>
+        <v>185</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>126</v>
+        <v>195</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>159</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>42</v>
+        <v>197</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="B24" t="s" s="2">
         <v>75</v>
@@ -1277,10 +1376,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>43</v>
+        <v>199</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>48</v>
+        <v>156</v>
       </c>
       <c r="C25" t="s" s="2">
         <v>5</v>
@@ -1288,65 +1387,65 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>172</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>93</v>
+        <v>200</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>105</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>173</v>
+        <v>201</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s" s="2">
         <v>13</v>
@@ -1354,10 +1453,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>161</v>
+        <v>202</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="C32" t="s" s="2">
         <v>13</v>
@@ -1365,10 +1464,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>65</v>
+        <v>204</v>
       </c>
       <c r="C33" t="s" s="2">
         <v>5</v>
@@ -1376,10 +1475,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>51</v>
+        <v>205</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s" s="2">
         <v>13</v>
@@ -1387,10 +1486,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>137</v>
+        <v>206</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s" s="2">
         <v>13</v>
@@ -1398,10 +1497,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>70</v>
+        <v>207</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s" s="2">
         <v>13</v>
@@ -1409,21 +1508,21 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>78</v>
+        <v>208</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>42</v>
+        <v>185</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s" s="2">
         <v>13</v>
@@ -1431,10 +1530,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>118</v>
+        <v>210</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>176</v>
+        <v>92</v>
       </c>
       <c r="C39" t="s" s="2">
         <v>13</v>
@@ -1442,21 +1541,21 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B40" t="s" s="2">
         <v>48</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>97</v>
+        <v>211</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>63</v>
+        <v>212</v>
       </c>
       <c r="C41" t="s" s="2">
         <v>13</v>
@@ -1464,111 +1563,34 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>158</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C43" t="s" s="2">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>177</v>
+        <v>61</v>
       </c>
       <c r="C44" t="s" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="B45" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="C45" t="s" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="B46" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="C46" t="s" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="B47" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="C47" t="s" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="B48" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="C48" t="s" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="B49" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="C49" t="s" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="B50" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="C50" t="s" s="2">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="B51" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="C51" t="s" s="2">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Before implementing the Strategy pattern for searchForLawyers function
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Reports.xlsx
+++ b/src/main/resources/baseFiles/excel/Reports.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="281">
   <si>
     <t>Firm</t>
   </si>
@@ -693,6 +693,210 @@
   </si>
   <si>
     <t>27s</t>
+  </si>
+  <si>
+    <t>K1 Chamber</t>
+  </si>
+  <si>
+    <t>59s</t>
+  </si>
+  <si>
+    <t>MAS Law</t>
+  </si>
+  <si>
+    <t>Nurmansyah And Muzdalifah</t>
+  </si>
+  <si>
+    <t>KISCH IP</t>
+  </si>
+  <si>
+    <t>Arthur Cox</t>
+  </si>
+  <si>
+    <t>02min 22s</t>
+  </si>
+  <si>
+    <t>45s</t>
+  </si>
+  <si>
+    <t>Thompson Dorfman Sweatman</t>
+  </si>
+  <si>
+    <t>Dompatent</t>
+  </si>
+  <si>
+    <t>Cobalt</t>
+  </si>
+  <si>
+    <t>01min 40s</t>
+  </si>
+  <si>
+    <t>Gitti And Partners</t>
+  </si>
+  <si>
+    <t>Helmsman</t>
+  </si>
+  <si>
+    <t>Ellisons Solicitors</t>
+  </si>
+  <si>
+    <t>Control Risks</t>
+  </si>
+  <si>
+    <t>03min 15s</t>
+  </si>
+  <si>
+    <t>Sangra</t>
+  </si>
+  <si>
+    <t>30s</t>
+  </si>
+  <si>
+    <t>Allens</t>
+  </si>
+  <si>
+    <t>03min 37s</t>
+  </si>
+  <si>
+    <t>Guantao Law</t>
+  </si>
+  <si>
+    <t>52min 08s</t>
+  </si>
+  <si>
+    <t>Oxera</t>
+  </si>
+  <si>
+    <t>02min 09s</t>
+  </si>
+  <si>
+    <t>Aera</t>
+  </si>
+  <si>
+    <t>Esche</t>
+  </si>
+  <si>
+    <t>SIRIUS</t>
+  </si>
+  <si>
+    <t>Huiye Law</t>
+  </si>
+  <si>
+    <t>Herbert Smith Freehills Kramer</t>
+  </si>
+  <si>
+    <t>Madrona</t>
+  </si>
+  <si>
+    <t>32s</t>
+  </si>
+  <si>
+    <t>03min 10s</t>
+  </si>
+  <si>
+    <t>02min 58s</t>
+  </si>
+  <si>
+    <t>Dentons</t>
+  </si>
+  <si>
+    <t>04min 27s</t>
+  </si>
+  <si>
+    <t>Clark Wilson</t>
+  </si>
+  <si>
+    <t>TEMPLARS</t>
+  </si>
+  <si>
+    <t>Tahota Law</t>
+  </si>
+  <si>
+    <t>Ramdas And Wong</t>
+  </si>
+  <si>
+    <t>Banki Haddock Fiora</t>
+  </si>
+  <si>
+    <t>Ellex</t>
+  </si>
+  <si>
+    <t>Horten</t>
+  </si>
+  <si>
+    <t>Macpherson Kelley</t>
+  </si>
+  <si>
+    <t>Zhongzi Law</t>
+  </si>
+  <si>
+    <t>Higgs And Johnson</t>
+  </si>
+  <si>
+    <t>GrandwayLaw</t>
+  </si>
+  <si>
+    <t>01min 57s</t>
+  </si>
+  <si>
+    <t>Blandy And Blandy</t>
+  </si>
+  <si>
+    <t>Carnelutti Law</t>
+  </si>
+  <si>
+    <t>46s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sherrards  </t>
+  </si>
+  <si>
+    <t>Roschier</t>
+  </si>
+  <si>
+    <t>Gornitzky And Co</t>
+  </si>
+  <si>
+    <t>Asafo And Co</t>
+  </si>
+  <si>
+    <t>DW Fox Tucker</t>
+  </si>
+  <si>
+    <t>Davies Ward Phillips And Vineberg</t>
+  </si>
+  <si>
+    <t>10min 01s</t>
+  </si>
+  <si>
+    <t>HY Leung And Co</t>
+  </si>
+  <si>
+    <t>BWB LLP</t>
+  </si>
+  <si>
+    <t>Santamarina And Steta</t>
+  </si>
+  <si>
+    <t>36s</t>
+  </si>
+  <si>
+    <t>Dale And Lessmann</t>
+  </si>
+  <si>
+    <t>EBN</t>
+  </si>
+  <si>
+    <t>01min 02s</t>
+  </si>
+  <si>
+    <t>Fangda Partners</t>
+  </si>
+  <si>
+    <t>02min 06s</t>
+  </si>
+  <si>
+    <t>Onsagers</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1302,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A350BCBC-CDDB-414C-9A72-BE6A09964F3F}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -1123,21 +1327,21 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>181</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>182</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>39</v>
+        <v>214</v>
       </c>
       <c r="C3" t="s" s="2">
         <v>32</v>
@@ -1145,10 +1349,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>150</v>
+        <v>215</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s" s="2">
         <v>13</v>
@@ -1156,10 +1360,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>149</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s" s="2">
         <v>54</v>
@@ -1167,21 +1371,21 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>183</v>
+        <v>216</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>55</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>185</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s" s="2">
         <v>13</v>
@@ -1189,21 +1393,21 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>160</v>
+        <v>218</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>61</v>
+        <v>219</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>47</v>
+        <v>220</v>
       </c>
       <c r="C9" t="s" s="2">
         <v>13</v>
@@ -1211,10 +1415,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>187</v>
+        <v>221</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s" s="2">
         <v>13</v>
@@ -1222,32 +1426,32 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>142</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>134</v>
+        <v>224</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>190</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C13" t="s" s="2">
         <v>13</v>
@@ -1255,10 +1459,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>192</v>
+        <v>225</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s" s="2">
         <v>13</v>
@@ -1266,21 +1470,21 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>107</v>
+        <v>182</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s" s="2">
         <v>13</v>
@@ -1288,21 +1492,21 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>88</v>
+        <v>226</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>172</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>145</v>
+        <v>227</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s" s="2">
         <v>13</v>
@@ -1310,21 +1514,21 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>127</v>
+        <v>228</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>177</v>
+        <v>229</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>193</v>
+        <v>230</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s" s="2">
         <v>13</v>
@@ -1332,21 +1536,21 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>194</v>
+        <v>147</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>195</v>
+        <v>232</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>46</v>
+        <v>233</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>13</v>
@@ -1354,54 +1558,54 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>196</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>197</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>54</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>75</v>
+        <v>235</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>199</v>
+        <v>236</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>156</v>
+        <v>237</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>106</v>
+        <v>238</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>121</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>91</v>
+        <v>239</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s" s="2">
         <v>13</v>
@@ -1409,21 +1613,21 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>154</v>
+        <v>241</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s" s="2">
         <v>13</v>
@@ -1431,21 +1635,21 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>201</v>
+        <v>242</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>157</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>61</v>
+        <v>185</v>
       </c>
       <c r="C31" t="s" s="2">
         <v>13</v>
@@ -1453,10 +1657,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>202</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>203</v>
+        <v>128</v>
       </c>
       <c r="C32" t="s" s="2">
         <v>13</v>
@@ -1464,32 +1668,32 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>204</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>205</v>
+        <v>243</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>46</v>
+        <v>159</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>206</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s" s="2">
         <v>13</v>
@@ -1497,65 +1701,65 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>207</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>56</v>
+        <v>244</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>208</v>
+        <v>93</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>185</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>209</v>
+        <v>103</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>210</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>92</v>
+        <v>245</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>48</v>
+        <v>246</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>212</v>
+        <v>248</v>
       </c>
       <c r="C41" t="s" s="2">
         <v>13</v>
@@ -1563,35 +1767,464 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>135</v>
+        <v>249</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>104</v>
+        <v>250</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>41</v>
+        <v>251</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="B46" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="C46" t="s" s="2">
         <v>5</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="B47" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="C47" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="B48" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="C48" t="s" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="C49" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="B51" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="C51" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="B52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="C52" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="B53" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="C53" t="s" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="B54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="C54" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="B55" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="C55" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="B56" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="C56" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="B57" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="C57" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="B58" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="C58" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="B59" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="C59" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="B60" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="C60" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="B61" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="C61" t="s" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="B62" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="C62" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="B63" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="C63" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="B64" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="C64" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="B65" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="C65" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="B66" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="C66" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="B67" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="C67" t="s" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="B68" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="C68" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="C69" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="B70" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="C70" t="s" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="B71" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="C71" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="B72" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="C72" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="B73" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="C73" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="B74" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="C74" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="B75" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="C75" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="B76" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="C76" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="B77" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="C77" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="B78" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="C78" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="B79" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="C79" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="B80" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="C80" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="B81" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="C81" t="s" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="B82" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="C82" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="B83" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="C83" t="s" s="2">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix in the classes, and more one time using it
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Reports.xlsx
+++ b/src/main/resources/baseFiles/excel/Reports.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="337">
   <si>
     <t>Firm</t>
   </si>
@@ -900,6 +900,171 @@
   </si>
   <si>
     <t>Chattertons</t>
+  </si>
+  <si>
+    <t>02min 52s</t>
+  </si>
+  <si>
+    <t>Meyer Köring</t>
+  </si>
+  <si>
+    <t>02min 36s</t>
+  </si>
+  <si>
+    <t>56s</t>
+  </si>
+  <si>
+    <t>01min 37s</t>
+  </si>
+  <si>
+    <t>Legance</t>
+  </si>
+  <si>
+    <t>02min 12s</t>
+  </si>
+  <si>
+    <t>55s</t>
+  </si>
+  <si>
+    <t>10min 46s</t>
+  </si>
+  <si>
+    <t>One Essex Court</t>
+  </si>
+  <si>
+    <t>CliffordChance</t>
+  </si>
+  <si>
+    <t>Garcia Bodan</t>
+  </si>
+  <si>
+    <t>Lewiss Silkin</t>
+  </si>
+  <si>
+    <t>02min 10s</t>
+  </si>
+  <si>
+    <t>Mourant</t>
+  </si>
+  <si>
+    <t>Keystone Law</t>
+  </si>
+  <si>
+    <t>01min 32s</t>
+  </si>
+  <si>
+    <t>Young List</t>
+  </si>
+  <si>
+    <t>15min 17s</t>
+  </si>
+  <si>
+    <t>Skadden</t>
+  </si>
+  <si>
+    <t>Morgan Lewis</t>
+  </si>
+  <si>
+    <t>KRBLaw</t>
+  </si>
+  <si>
+    <t>Kuri Breña</t>
+  </si>
+  <si>
+    <t>ENS Africa</t>
+  </si>
+  <si>
+    <t>LonganLaw</t>
+  </si>
+  <si>
+    <t>05min 11s</t>
+  </si>
+  <si>
+    <t>04min 40s</t>
+  </si>
+  <si>
+    <t>Nader Hayaux And Goebel</t>
+  </si>
+  <si>
+    <t>Legalis</t>
+  </si>
+  <si>
+    <t>Prasad And Company</t>
+  </si>
+  <si>
+    <t>01min 00s</t>
+  </si>
+  <si>
+    <t>Mishcon Karas</t>
+  </si>
+  <si>
+    <t>Baumgartners</t>
+  </si>
+  <si>
+    <t>22min 46s</t>
+  </si>
+  <si>
+    <t>01min 41s</t>
+  </si>
+  <si>
+    <t>Langseth Advokat</t>
+  </si>
+  <si>
+    <t>02min 20s</t>
+  </si>
+  <si>
+    <t>01min 55s</t>
+  </si>
+  <si>
+    <t>Ibañez Parkman</t>
+  </si>
+  <si>
+    <t>TCLaw</t>
+  </si>
+  <si>
+    <t>01min 08s</t>
+  </si>
+  <si>
+    <t>01min 56s</t>
+  </si>
+  <si>
+    <t>52s</t>
+  </si>
+  <si>
+    <t>Lex Caribbean</t>
+  </si>
+  <si>
+    <t>Laszczuk And Wspolnicy</t>
+  </si>
+  <si>
+    <t>01min 54s</t>
+  </si>
+  <si>
+    <t>00s</t>
+  </si>
+  <si>
+    <t>GÖRG</t>
+  </si>
+  <si>
+    <t>02min 00s</t>
+  </si>
+  <si>
+    <t>05min 02s</t>
+  </si>
+  <si>
+    <t>01min 07s</t>
+  </si>
+  <si>
+    <t>Gadens</t>
+  </si>
+  <si>
+    <t>06min 49s</t>
+  </si>
+  <si>
+    <t>01min 26s</t>
+  </si>
+  <si>
+    <t>02min 50s</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A350BCBC-CDDB-414C-9A72-BE6A09964F3F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -1328,39 +1493,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>111</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixes in the classes, added more firms, updated the log files
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Reports.xlsx
+++ b/src/main/resources/baseFiles/excel/Reports.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2565" uniqueCount="370">
   <si>
     <t>Firm</t>
   </si>
@@ -1143,6 +1143,27 @@
   </si>
   <si>
     <t>Grandway Law</t>
+  </si>
+  <si>
+    <t>04min 17s</t>
+  </si>
+  <si>
+    <t>01min 23s</t>
+  </si>
+  <si>
+    <t>04min 44s</t>
+  </si>
+  <si>
+    <t>48s</t>
+  </si>
+  <si>
+    <t>01min 34s</t>
+  </si>
+  <si>
+    <t>09min 25s</t>
+  </si>
+  <si>
+    <t>58s</t>
   </si>
 </sst>
 </file>
@@ -1548,7 +1569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A350BCBC-CDDB-414C-9A72-BE6A09964F3F}">
-  <dimension ref="A1:C129"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -1573,54 +1594,54 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>294</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>335</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>54</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>106</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>204</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>47</v>
+        <v>220</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>222</v>
+        <v>349</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>40</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s" s="2">
         <v>13</v>
@@ -1628,76 +1649,76 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>215</v>
+        <v>351</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>46</v>
+        <v>312</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>230</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>42</v>
+        <v>312</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>296</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>136</v>
+        <v>312</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>56</v>
+        <v>274</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>261</v>
+        <v>306</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>185</v>
+        <v>312</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>304</v>
+        <v>161</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>337</v>
+        <v>227</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>338</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s" s="2">
         <v>13</v>
@@ -1705,10 +1726,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>156</v>
+        <v>312</v>
       </c>
       <c r="C14" t="s" s="2">
         <v>32</v>
@@ -1716,43 +1737,43 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>301</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>185</v>
+        <v>312</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>23</v>
+        <v>267</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>339</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>256</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>134</v>
+        <v>312</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>196</v>
+        <v>348</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>263</v>
+        <v>312</v>
       </c>
       <c r="C18" t="s" s="2">
         <v>32</v>
@@ -1760,79 +1781,79 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>340</v>
+        <v>278</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>341</v>
+        <v>312</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>25</v>
+        <v>216</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>342</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>104</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>152</v>
+        <v>362</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>343</v>
+        <v>312</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>120</v>
+        <v>242</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>344</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>79</v>
+        <v>312</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>149</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>338</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26">
@@ -1840,7 +1861,7 @@
         <v>313</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s" s="2">
         <v>32</v>
@@ -1848,65 +1869,65 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>171</v>
+        <v>358</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>43</v>
+        <v>257</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>54</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>345</v>
+        <v>228</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>185</v>
+        <v>369</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s" s="2">
         <v>52</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>192</v>
+        <v>143</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s" s="2">
         <v>32</v>
@@ -1914,21 +1935,21 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>209</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>231</v>
+        <v>312</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>202</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>46</v>
+        <v>312</v>
       </c>
       <c r="C34" t="s" s="2">
         <v>13</v>
@@ -1936,32 +1957,32 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>346</v>
+        <v>119</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>159</v>
+        <v>47</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>62</v>
+        <v>196</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>52</v>
+        <v>191</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>291</v>
+        <v>213</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>347</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s" s="2">
         <v>32</v>
@@ -1969,10 +1990,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>321</v>
+        <v>192</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>328</v>
+        <v>263</v>
       </c>
       <c r="C38" t="s" s="2">
         <v>32</v>
@@ -1980,10 +2001,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>129</v>
+        <v>321</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="C39" t="s" s="2">
         <v>32</v>
@@ -1991,992 +2012,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>328</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="B41" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C41" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s" s="2">
-        <v>130</v>
-      </c>
-      <c r="B42" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C42" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="B43" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C43" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="B44" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C44" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="B45" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C45" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="B46" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C46" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="B47" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C47" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="B48" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C48" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="B49" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C49" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="B50" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C50" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s" s="2">
-        <v>349</v>
-      </c>
-      <c r="B51" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C51" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="B52" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C52" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="B53" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C53" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="B54" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C54" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="B55" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C55" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="B56" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C56" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="B57" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C57" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="B58" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C58" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="B59" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C59" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="B60" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C60" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="B61" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C61" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="B62" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C62" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="B63" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C63" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="B64" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C64" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="B65" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C65" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="B66" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C66" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="B67" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C67" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="B68" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C68" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="B69" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C69" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="B70" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C70" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="B71" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C71" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="B72" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C72" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="B73" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C73" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="B74" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C74" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="B75" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C75" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="B76" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C76" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="B77" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C77" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="B78" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C78" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="B79" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C79" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="B80" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C80" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="B81" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C81" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="B82" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C82" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="B83" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C83" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="B84" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C84" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="B85" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C85" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="B86" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C86" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="B87" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C87" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="B88" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C88" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="B89" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C89" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="B90" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C90" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="B91" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C91" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="B92" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C92" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="B93" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C93" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="B94" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C94" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="B95" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C95" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="B96" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C96" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="B97" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C97" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B98" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C98" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="B99" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C99" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="B100" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C100" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="B101" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C101" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="B102" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C102" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="B103" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C103" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="B104" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C104" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="B105" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C105" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="B106" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C106" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="B107" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C107" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="B108" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C108" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="B109" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C109" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="B110" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C110" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="B111" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C111" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="B112" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C112" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="B113" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C113" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="s" s="2">
-        <v>326</v>
-      </c>
-      <c r="B114" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C114" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="B115" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C115" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="B116" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C116" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="B117" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C117" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="B118" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C118" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="B119" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C119" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="B120" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C120" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="B121" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C121" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="B122" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C122" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="s" s="2">
-        <v>362</v>
-      </c>
-      <c r="B123" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C123" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="B124" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C124" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="B125" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C125" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="B126" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C126" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="B127" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C127" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="B128" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C128" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="B129" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C129" t="s" s="2">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes and more firms
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Reports.xlsx
+++ b/src/main/resources/baseFiles/excel/Reports.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="151">
   <si>
     <t>Firm</t>
   </si>
@@ -222,6 +222,264 @@
   </si>
   <si>
     <t>48s</t>
+  </si>
+  <si>
+    <t>05s</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Winston And Strawn</t>
+  </si>
+  <si>
+    <t>09s</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Matheson</t>
+  </si>
+  <si>
+    <t>Krogerus</t>
+  </si>
+  <si>
+    <t>Aron Tadmor Levy</t>
+  </si>
+  <si>
+    <t>59s</t>
+  </si>
+  <si>
+    <t>Dentons</t>
+  </si>
+  <si>
+    <t>Hakun Law</t>
+  </si>
+  <si>
+    <t>01min 20s</t>
+  </si>
+  <si>
+    <t>27s</t>
+  </si>
+  <si>
+    <t>Hans Offia And Associates</t>
+  </si>
+  <si>
+    <t>Prinz &amp; Partner</t>
+  </si>
+  <si>
+    <t>Ogier</t>
+  </si>
+  <si>
+    <t>53s</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Arthur Cox</t>
+  </si>
+  <si>
+    <t>03min 59s</t>
+  </si>
+  <si>
+    <t>BCF Law</t>
+  </si>
+  <si>
+    <t>BNT</t>
+  </si>
+  <si>
+    <t>DBHLaw</t>
+  </si>
+  <si>
+    <t>25s</t>
+  </si>
+  <si>
+    <t>37s</t>
+  </si>
+  <si>
+    <t>Foyen</t>
+  </si>
+  <si>
+    <t>JGSA</t>
+  </si>
+  <si>
+    <t>Appleby Global</t>
+  </si>
+  <si>
+    <t>Bennett Jones</t>
+  </si>
+  <si>
+    <t>Horten</t>
+  </si>
+  <si>
+    <t>Tahota Law</t>
+  </si>
+  <si>
+    <t>Nader Hayaux And Goebel</t>
+  </si>
+  <si>
+    <t>Dittmar And Indrenius</t>
+  </si>
+  <si>
+    <t>44s</t>
+  </si>
+  <si>
+    <t>Thommessen</t>
+  </si>
+  <si>
+    <t>AOil</t>
+  </si>
+  <si>
+    <t>10s</t>
+  </si>
+  <si>
+    <t>Chattertons</t>
+  </si>
+  <si>
+    <t>08s</t>
+  </si>
+  <si>
+    <t>Kromann Reumert</t>
+  </si>
+  <si>
+    <t>26s</t>
+  </si>
+  <si>
+    <t>Guantao Law</t>
+  </si>
+  <si>
+    <t>03min 41s</t>
+  </si>
+  <si>
+    <t>MSP</t>
+  </si>
+  <si>
+    <t>Santamarina And Steta</t>
+  </si>
+  <si>
+    <t>31s</t>
+  </si>
+  <si>
+    <t>AC&amp;R</t>
+  </si>
+  <si>
+    <t>BWB LLP</t>
+  </si>
+  <si>
+    <t>Ramdas And Wong</t>
+  </si>
+  <si>
+    <t>Kolster</t>
+  </si>
+  <si>
+    <t>16s</t>
+  </si>
+  <si>
+    <t>Viering Jentschura And Partner</t>
+  </si>
+  <si>
+    <t>20s</t>
+  </si>
+  <si>
+    <t>Reliance Corporate Advisors</t>
+  </si>
+  <si>
+    <t>01s</t>
+  </si>
+  <si>
+    <t>Kondrat</t>
+  </si>
+  <si>
+    <t>49s</t>
+  </si>
+  <si>
+    <t>Meyer Köring</t>
+  </si>
+  <si>
+    <t>Liedekerke</t>
+  </si>
+  <si>
+    <t>06s</t>
+  </si>
+  <si>
+    <t>Steinmetz Haring Gurman</t>
+  </si>
+  <si>
+    <t>Laszczuk And Wspolnicy</t>
+  </si>
+  <si>
+    <t>Gomez Acebo And Pombo</t>
+  </si>
+  <si>
+    <t>01min 01s</t>
+  </si>
+  <si>
+    <t>01min 13s</t>
+  </si>
+  <si>
+    <t>WikborgRein</t>
+  </si>
+  <si>
+    <t>William Fry</t>
+  </si>
+  <si>
+    <t>Belgravia</t>
+  </si>
+  <si>
+    <t>Peter And Kim</t>
+  </si>
+  <si>
+    <t>Carnelutti Law</t>
+  </si>
+  <si>
+    <t>Sherrards</t>
+  </si>
+  <si>
+    <t>Huiye Law</t>
+  </si>
+  <si>
+    <t>Wolf Theiss</t>
+  </si>
+  <si>
+    <t>Walkers</t>
+  </si>
+  <si>
+    <t>Dale And Lessmann</t>
+  </si>
+  <si>
+    <t>Banki Haddock Fiora</t>
+  </si>
+  <si>
+    <t>Flügel Preissner</t>
+  </si>
+  <si>
+    <t>EProint</t>
+  </si>
+  <si>
+    <t>03min 25s</t>
+  </si>
+  <si>
+    <t>24s</t>
+  </si>
+  <si>
+    <t>Ashurst</t>
+  </si>
+  <si>
+    <t>Gadens</t>
+  </si>
+  <si>
+    <t>Latham And Watkins</t>
+  </si>
+  <si>
+    <t>02min 15s</t>
+  </si>
+  <si>
+    <t>HFW</t>
+  </si>
+  <si>
+    <t>01min 22s</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1474,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1224,8 +1482,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="3" width="27.6634615384615" style="1" customWidth="1"/>
-    <col min="4" max="8" width="8.88461538461539" customWidth="1"/>
+    <col min="1" max="3" customWidth="true" style="1" width="27.6634615384615"/>
+    <col min="4" max="8" customWidth="true" width="8.88461538461539"/>
   </cols>
   <sheetData>
     <row r="1" ht="23.2" spans="1:3">
@@ -1239,378 +1497,873 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="1">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="1">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s" s="1">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="1">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="1">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s" s="1">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="1">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="1">
+        <v>75</v>
+      </c>
+      <c r="B8" t="s" s="1">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="1">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s" s="1">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="1">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s" s="1">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="1">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="1">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="C12" t="s" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="1">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s" s="1">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="1">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s" s="1">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="1">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="1">
+        <v>87</v>
+      </c>
+      <c r="B17" t="s" s="1">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="1">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s" s="1">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="1">
+        <v>90</v>
+      </c>
+      <c r="B19" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="1">
+        <v>91</v>
+      </c>
+      <c r="B20" t="s" s="1">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="1">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="1">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s" s="1">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="1">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="1">
+        <v>93</v>
+      </c>
+      <c r="B24" t="s" s="1">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="1">
+        <v>94</v>
+      </c>
+      <c r="B25" t="s" s="1">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="1">
+        <v>95</v>
+      </c>
+      <c r="B26" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="B27" t="s" s="1">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="1">
+        <v>97</v>
+      </c>
+      <c r="B28" t="s" s="1">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="1">
+        <v>99</v>
+      </c>
+      <c r="B29" t="s" s="1">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="1">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s" s="1">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="1">
+        <v>100</v>
+      </c>
+      <c r="B31" t="s" s="1">
+        <v>101</v>
+      </c>
+      <c r="C31" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="1">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s" s="1">
+        <v>103</v>
+      </c>
+      <c r="C32" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="1">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s" s="1">
+        <v>105</v>
+      </c>
+      <c r="C33" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="1">
+        <v>106</v>
+      </c>
+      <c r="B34" t="s" s="1">
+        <v>107</v>
+      </c>
+      <c r="C34" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="1">
+        <v>108</v>
+      </c>
+      <c r="B35" t="s" s="1">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="1">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="1">
+        <v>109</v>
+      </c>
+      <c r="B38" t="s" s="1">
+        <v>110</v>
+      </c>
+      <c r="C38" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="1">
+        <v>111</v>
+      </c>
+      <c r="B39" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="1">
+        <v>112</v>
+      </c>
+      <c r="B40" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="1">
+        <v>113</v>
+      </c>
+      <c r="B41" t="s" s="1">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="1">
+        <v>114</v>
+      </c>
+      <c r="B42" t="s" s="1">
+        <v>115</v>
+      </c>
+      <c r="C42" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="1">
+        <v>116</v>
+      </c>
+      <c r="B43" t="s" s="1">
+        <v>117</v>
+      </c>
+      <c r="C43" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="1">
+        <v>118</v>
+      </c>
+      <c r="B44" t="s" s="1">
+        <v>119</v>
+      </c>
+      <c r="C44" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="1">
+        <v>55</v>
+      </c>
+      <c r="B45" t="s" s="1">
+        <v>56</v>
+      </c>
+      <c r="C45" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="1">
+        <v>120</v>
+      </c>
+      <c r="B46" t="s" s="1">
+        <v>77</v>
+      </c>
+      <c r="C46" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="1">
+        <v>63</v>
+      </c>
+      <c r="B47" t="s" s="1">
+        <v>121</v>
+      </c>
+      <c r="C47" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="1">
+        <v>122</v>
+      </c>
+      <c r="B48" t="s" s="1">
+        <v>105</v>
+      </c>
+      <c r="C48" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="1">
+        <v>123</v>
+      </c>
+      <c r="B49" t="s" s="1">
+        <v>124</v>
+      </c>
+      <c r="C49" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="1">
+        <v>125</v>
+      </c>
+      <c r="B50" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C50" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="1">
+        <v>126</v>
+      </c>
+      <c r="B51" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="C51" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="1">
+        <v>127</v>
+      </c>
+      <c r="B52" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="B53" t="s" s="1">
+        <v>128</v>
+      </c>
+      <c r="C53" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="B54" t="s" s="1">
+        <v>89</v>
+      </c>
+      <c r="C54" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="1">
+        <v>61</v>
+      </c>
+      <c r="B55" t="s" s="1">
+        <v>129</v>
+      </c>
+      <c r="C55" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="1">
+        <v>130</v>
+      </c>
+      <c r="B56" t="s" s="1">
+        <v>46</v>
+      </c>
+      <c r="C56" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="1">
+        <v>131</v>
+      </c>
+      <c r="B57" t="s" s="1">
+        <v>110</v>
+      </c>
+      <c r="C57" t="s" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="1">
+        <v>24</v>
+      </c>
+      <c r="B58" t="s" s="1">
+        <v>31</v>
+      </c>
+      <c r="C58" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="1">
+        <v>132</v>
+      </c>
+      <c r="B59" t="s" s="1">
+        <v>124</v>
+      </c>
+      <c r="C59" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="1">
+        <v>133</v>
+      </c>
+      <c r="B60" t="s" s="1">
+        <v>11</v>
+      </c>
+      <c r="C60" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="1">
+        <v>51</v>
+      </c>
+      <c r="B61" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="C61" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="B62" t="s" s="1">
+        <v>88</v>
+      </c>
+      <c r="C62" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="1">
+        <v>134</v>
+      </c>
+      <c r="B63" t="s" s="1">
+        <v>31</v>
+      </c>
+      <c r="C63" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="1">
+        <v>135</v>
+      </c>
+      <c r="B64" t="s" s="1">
+        <v>110</v>
+      </c>
+      <c r="C64" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="1">
+        <v>136</v>
+      </c>
+      <c r="B65" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="C65" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="1">
+        <v>137</v>
+      </c>
+      <c r="B66" t="s" s="1">
+        <v>31</v>
+      </c>
+      <c r="C66" t="s" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="1">
+        <v>138</v>
+      </c>
+      <c r="B67" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="C67" t="s" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="1">
+        <v>139</v>
+      </c>
+      <c r="B68" t="s" s="1">
+        <v>68</v>
+      </c>
+      <c r="C68" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="B69" t="s" s="1">
+        <v>44</v>
+      </c>
+      <c r="C69" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="B70" t="s" s="1">
+        <v>124</v>
+      </c>
+      <c r="C70" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="1">
+        <v>141</v>
+      </c>
+      <c r="B71" t="s" s="1">
+        <v>101</v>
+      </c>
+      <c r="C71" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="1">
+        <v>142</v>
+      </c>
+      <c r="B72" t="s" s="1">
+        <v>143</v>
+      </c>
+      <c r="C72" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="C73" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+      <c r="B74" t="s" s="1">
+        <v>144</v>
+      </c>
+      <c r="C74" t="s" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="1">
+        <v>145</v>
+      </c>
+      <c r="B75" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="C75" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="1">
+        <v>146</v>
+      </c>
+      <c r="B76" t="s" s="1">
+        <v>84</v>
+      </c>
+      <c r="C76" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="B77" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C77" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="1">
+        <v>147</v>
+      </c>
+      <c r="B78" t="s" s="1">
+        <v>148</v>
+      </c>
+      <c r="C78" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="1">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B79" t="s" s="1">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>5</v>
+      <c r="C79" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="1">
+        <v>149</v>
+      </c>
+      <c r="B80" t="s" s="1">
+        <v>150</v>
+      </c>
+      <c r="C80" t="s" s="1">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More one time using it
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Reports.xlsx
+++ b/src/main/resources/baseFiles/excel/Reports.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="331">
   <si>
     <t>Firm</t>
   </si>
@@ -928,6 +928,99 @@
   </si>
   <si>
     <t>39s</t>
+  </si>
+  <si>
+    <t>Nielsen Nørager</t>
+  </si>
+  <si>
+    <t>04s</t>
+  </si>
+  <si>
+    <t>LEXIA</t>
+  </si>
+  <si>
+    <t>Moroğlu Arseven</t>
+  </si>
+  <si>
+    <t>01min 27s</t>
+  </si>
+  <si>
+    <t>H-F &amp; Co</t>
+  </si>
+  <si>
+    <t>Secretariat</t>
+  </si>
+  <si>
+    <t>03min 04s</t>
+  </si>
+  <si>
+    <t>METIDA</t>
+  </si>
+  <si>
+    <t>Knezović &amp; Associates</t>
+  </si>
+  <si>
+    <t>Cuatrecasas</t>
+  </si>
+  <si>
+    <t>01min 35s</t>
+  </si>
+  <si>
+    <t>Loopstra Nixon</t>
+  </si>
+  <si>
+    <t>32s</t>
+  </si>
+  <si>
+    <t>Joksovic Stojanovic &amp; Partners</t>
+  </si>
+  <si>
+    <t>Morris Law</t>
+  </si>
+  <si>
+    <t>01min 10s</t>
+  </si>
+  <si>
+    <t>Joffe &amp; Associés</t>
+  </si>
+  <si>
+    <t>Robortella e Peres</t>
+  </si>
+  <si>
+    <t>Molinari</t>
+  </si>
+  <si>
+    <t>Lindahl</t>
+  </si>
+  <si>
+    <t>Roca Junyent</t>
+  </si>
+  <si>
+    <t>02min 59s</t>
+  </si>
+  <si>
+    <t>Mazanti-Andersen</t>
+  </si>
+  <si>
+    <t>01min 24s</t>
+  </si>
+  <si>
+    <t>McConnell Valdés</t>
+  </si>
+  <si>
+    <t>Nelson Wilians &amp; Advogados</t>
+  </si>
+  <si>
+    <t>03min 35s</t>
+  </si>
+  <si>
+    <t>01min 33s</t>
+  </si>
+  <si>
+    <t>01min 05s</t>
+  </si>
+  <si>
+    <t>Lambadarios Law</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Before checkign if the validation of global is working
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/Reports.xlsx
+++ b/src/main/resources/baseFiles/excel/Reports.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3768" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4467" uniqueCount="529">
   <si>
     <t>Firm</t>
   </si>
@@ -1606,6 +1606,15 @@
   </si>
   <si>
     <t>02min 56s</t>
+  </si>
+  <si>
+    <t>02min 35s</t>
+  </si>
+  <si>
+    <t>02min 30s</t>
+  </si>
+  <si>
+    <t>02min 06s</t>
   </si>
 </sst>
 </file>
@@ -2593,7 +2602,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C124"/>
+  <dimension ref="A1:C234"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="99" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C35"/>
@@ -2618,43 +2627,43 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="1">
-        <v>358</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s" s="1">
-        <v>276</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>5</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="1">
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s" s="1">
-        <v>69</v>
+        <v>267</v>
       </c>
       <c r="C3" t="s" s="1">
-        <v>271</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="1">
-        <v>199</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
-        <v>245</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s" s="1">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="C5" t="s" s="1">
         <v>271</v>
@@ -2662,10 +2671,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
-        <v>226</v>
+        <v>464</v>
       </c>
       <c r="B6" t="s" s="1">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="C6" t="s" s="1">
         <v>271</v>
@@ -2673,10 +2682,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
-        <v>510</v>
+        <v>381</v>
       </c>
       <c r="B7" t="s" s="1">
-        <v>13</v>
+        <v>301</v>
       </c>
       <c r="C7" t="s" s="1">
         <v>271</v>
@@ -2684,7 +2693,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
-        <v>201</v>
+        <v>408</v>
       </c>
       <c r="B8" t="s" s="1">
         <v>289</v>
@@ -2695,10 +2704,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
-        <v>435</v>
+        <v>335</v>
       </c>
       <c r="B9" t="s" s="1">
-        <v>57</v>
+        <v>301</v>
       </c>
       <c r="C9" t="s" s="1">
         <v>271</v>
@@ -2706,10 +2715,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
-        <v>444</v>
+        <v>261</v>
       </c>
       <c r="B10" t="s" s="1">
-        <v>267</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s" s="1">
         <v>5</v>
@@ -2717,10 +2726,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
-        <v>353</v>
+        <v>260</v>
       </c>
       <c r="B11" t="s" s="1">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C11" t="s" s="1">
         <v>271</v>
@@ -2728,54 +2737,54 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
-        <v>511</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s" s="1">
-        <v>288</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s" s="1">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="1">
-        <v>229</v>
+        <v>346</v>
       </c>
       <c r="B13" t="s" s="1">
-        <v>313</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s" s="1">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="1">
-        <v>148</v>
+        <v>208</v>
       </c>
       <c r="B14" t="s" s="1">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="1">
-        <v>315</v>
+        <v>144</v>
       </c>
       <c r="B15" t="s" s="1">
-        <v>283</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="1">
-        <v>225</v>
+        <v>183</v>
       </c>
       <c r="B16" t="s" s="1">
-        <v>116</v>
+        <v>301</v>
       </c>
       <c r="C16" t="s" s="1">
         <v>271</v>
@@ -2783,21 +2792,21 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
-        <v>163</v>
+        <v>308</v>
       </c>
       <c r="B17" t="s" s="1">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s" s="1">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
-        <v>59</v>
+        <v>429</v>
       </c>
       <c r="B18" t="s" s="1">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>271</v>
@@ -2805,21 +2814,21 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
-        <v>203</v>
+        <v>466</v>
       </c>
       <c r="B19" t="s" s="1">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
-        <v>421</v>
+        <v>379</v>
       </c>
       <c r="B20" t="s" s="1">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C20" t="s" s="1">
         <v>271</v>
@@ -2827,10 +2836,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
-        <v>115</v>
+        <v>176</v>
       </c>
       <c r="B21" t="s" s="1">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s" s="1">
         <v>270</v>
@@ -2838,7 +2847,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
-        <v>446</v>
+        <v>215</v>
       </c>
       <c r="B22" t="s" s="1">
         <v>276</v>
@@ -2849,10 +2858,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
-        <v>170</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s" s="1">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s" s="1">
         <v>271</v>
@@ -2860,10 +2869,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
-        <v>308</v>
+        <v>353</v>
       </c>
       <c r="B24" t="s" s="1">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s" s="1">
         <v>271</v>
@@ -2871,10 +2880,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B25" t="s" s="1">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="C25" t="s" s="1">
         <v>271</v>
@@ -2882,10 +2891,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
-        <v>215</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s" s="1">
-        <v>281</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s" s="1">
         <v>271</v>
@@ -2893,10 +2902,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="1">
-        <v>401</v>
+        <v>245</v>
       </c>
       <c r="B27" t="s" s="1">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s" s="1">
         <v>271</v>
@@ -2904,10 +2913,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="1">
-        <v>65</v>
+        <v>501</v>
       </c>
       <c r="B28" t="s" s="1">
-        <v>289</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s" s="1">
         <v>271</v>
@@ -2915,10 +2924,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="1">
-        <v>493</v>
+        <v>435</v>
       </c>
       <c r="B29" t="s" s="1">
-        <v>301</v>
+        <v>392</v>
       </c>
       <c r="C29" t="s" s="1">
         <v>271</v>
@@ -2926,10 +2935,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
-        <v>300</v>
+        <v>483</v>
       </c>
       <c r="B30" t="s" s="1">
-        <v>34</v>
+        <v>337</v>
       </c>
       <c r="C30" t="s" s="1">
         <v>271</v>
@@ -2937,21 +2946,21 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="1">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="B31" t="s" s="1">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="1">
-        <v>513</v>
+        <v>233</v>
       </c>
       <c r="B32" t="s" s="1">
-        <v>286</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s" s="1">
         <v>271</v>
@@ -2959,10 +2968,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="1">
-        <v>70</v>
+        <v>519</v>
       </c>
       <c r="B33" t="s" s="1">
-        <v>301</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s" s="1">
         <v>271</v>
@@ -2970,10 +2979,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="1">
-        <v>345</v>
+        <v>495</v>
       </c>
       <c r="B34" t="s" s="1">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="C34" t="s" s="1">
         <v>271</v>
@@ -2981,32 +2990,32 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="1">
-        <v>42</v>
+        <v>198</v>
       </c>
       <c r="B35" t="s" s="1">
-        <v>280</v>
+        <v>494</v>
       </c>
       <c r="C35" t="s" s="1">
-        <v>271</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="1">
-        <v>176</v>
+        <v>244</v>
       </c>
       <c r="B36" t="s" s="1">
-        <v>84</v>
+        <v>301</v>
       </c>
       <c r="C36" t="s" s="1">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="1">
-        <v>424</v>
+        <v>377</v>
       </c>
       <c r="B37" t="s" s="1">
-        <v>301</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s" s="1">
         <v>271</v>
@@ -3014,43 +3023,43 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="1">
-        <v>330</v>
+        <v>258</v>
       </c>
       <c r="B38" t="s" s="1">
-        <v>72</v>
+        <v>491</v>
       </c>
       <c r="C38" t="s" s="1">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="1">
-        <v>514</v>
+        <v>444</v>
       </c>
       <c r="B39" t="s" s="1">
-        <v>286</v>
+        <v>111</v>
       </c>
       <c r="C39" t="s" s="1">
-        <v>271</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="1">
-        <v>318</v>
+        <v>480</v>
       </c>
       <c r="B40" t="s" s="1">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="1">
-        <v>310</v>
+        <v>168</v>
       </c>
       <c r="B41" t="s" s="1">
-        <v>515</v>
+        <v>337</v>
       </c>
       <c r="C41" t="s" s="1">
         <v>271</v>
@@ -3058,32 +3067,32 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="1">
-        <v>236</v>
+        <v>161</v>
       </c>
       <c r="B42" t="s" s="1">
-        <v>34</v>
+        <v>313</v>
       </c>
       <c r="C42" t="s" s="1">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="1">
-        <v>219</v>
+        <v>395</v>
       </c>
       <c r="B43" t="s" s="1">
-        <v>316</v>
+        <v>289</v>
       </c>
       <c r="C43" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="1">
-        <v>205</v>
+        <v>522</v>
       </c>
       <c r="B44" t="s" s="1">
-        <v>45</v>
+        <v>284</v>
       </c>
       <c r="C44" t="s" s="1">
         <v>271</v>
@@ -3091,10 +3100,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="1">
-        <v>173</v>
+        <v>436</v>
       </c>
       <c r="B45" t="s" s="1">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C45" t="s" s="1">
         <v>271</v>
@@ -3102,21 +3111,21 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="1">
-        <v>516</v>
+        <v>149</v>
       </c>
       <c r="B46" t="s" s="1">
-        <v>4</v>
+        <v>526</v>
       </c>
       <c r="C46" t="s" s="1">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="1">
-        <v>351</v>
+        <v>488</v>
       </c>
       <c r="B47" t="s" s="1">
-        <v>517</v>
+        <v>337</v>
       </c>
       <c r="C47" t="s" s="1">
         <v>271</v>
@@ -3124,32 +3133,32 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="1">
-        <v>46</v>
+        <v>421</v>
       </c>
       <c r="B48" t="s" s="1">
-        <v>289</v>
+        <v>4</v>
       </c>
       <c r="C48" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="1">
-        <v>518</v>
+        <v>187</v>
       </c>
       <c r="B49" t="s" s="1">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="C49" t="s" s="1">
-        <v>271</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="1">
-        <v>97</v>
+        <v>356</v>
       </c>
       <c r="B50" t="s" s="1">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s" s="1">
         <v>271</v>
@@ -3157,43 +3166,43 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="1">
-        <v>371</v>
+        <v>474</v>
       </c>
       <c r="B51" t="s" s="1">
-        <v>279</v>
+        <v>45</v>
       </c>
       <c r="C51" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="1">
-        <v>434</v>
+        <v>228</v>
       </c>
       <c r="B52" t="s" s="1">
         <v>25</v>
       </c>
       <c r="C52" t="s" s="1">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="1">
-        <v>119</v>
+        <v>399</v>
       </c>
       <c r="B53" t="s" s="1">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="1">
-        <v>336</v>
+        <v>225</v>
       </c>
       <c r="B54" t="s" s="1">
-        <v>337</v>
+        <v>45</v>
       </c>
       <c r="C54" t="s" s="1">
         <v>271</v>
@@ -3201,21 +3210,21 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="1">
-        <v>179</v>
+        <v>382</v>
       </c>
       <c r="B55" t="s" s="1">
-        <v>281</v>
+        <v>66</v>
       </c>
       <c r="C55" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="1">
-        <v>454</v>
+        <v>210</v>
       </c>
       <c r="B56" t="s" s="1">
-        <v>27</v>
+        <v>299</v>
       </c>
       <c r="C56" t="s" s="1">
         <v>271</v>
@@ -3223,21 +3232,21 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="1">
-        <v>172</v>
+        <v>259</v>
       </c>
       <c r="B57" t="s" s="1">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C57" t="s" s="1">
-        <v>271</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="1">
-        <v>317</v>
+        <v>87</v>
       </c>
       <c r="B58" t="s" s="1">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C58" t="s" s="1">
         <v>271</v>
@@ -3245,21 +3254,21 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="1">
-        <v>259</v>
+        <v>68</v>
       </c>
       <c r="B59" t="s" s="1">
-        <v>111</v>
+        <v>289</v>
       </c>
       <c r="C59" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="1">
-        <v>230</v>
+        <v>424</v>
       </c>
       <c r="B60" t="s" s="1">
-        <v>286</v>
+        <v>34</v>
       </c>
       <c r="C60" t="s" s="1">
         <v>271</v>
@@ -3267,29 +3276,29 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="1">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="B61" t="s" s="1">
-        <v>34</v>
+        <v>286</v>
       </c>
       <c r="C61" t="s" s="1">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="1">
-        <v>228</v>
+        <v>428</v>
       </c>
       <c r="B62" t="s" s="1">
         <v>52</v>
       </c>
       <c r="C62" t="s" s="1">
-        <v>268</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="1">
-        <v>423</v>
+        <v>162</v>
       </c>
       <c r="B63" t="s" s="1">
         <v>7</v>
@@ -3300,10 +3309,10 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="1">
-        <v>343</v>
+        <v>518</v>
       </c>
       <c r="B64" t="s" s="1">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C64" t="s" s="1">
         <v>271</v>
@@ -3311,10 +3320,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="1">
-        <v>410</v>
+        <v>181</v>
       </c>
       <c r="B65" t="s" s="1">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="C65" t="s" s="1">
         <v>271</v>
@@ -3322,10 +3331,10 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="1">
-        <v>252</v>
+        <v>422</v>
       </c>
       <c r="B66" t="s" s="1">
-        <v>45</v>
+        <v>273</v>
       </c>
       <c r="C66" t="s" s="1">
         <v>271</v>
@@ -3333,10 +3342,10 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="1">
-        <v>261</v>
+        <v>153</v>
       </c>
       <c r="B67" t="s" s="1">
-        <v>72</v>
+        <v>289</v>
       </c>
       <c r="C67" t="s" s="1">
         <v>5</v>
@@ -3344,10 +3353,10 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="1">
-        <v>366</v>
+        <v>476</v>
       </c>
       <c r="B68" t="s" s="1">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="C68" t="s" s="1">
         <v>271</v>
@@ -3355,10 +3364,10 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="1">
-        <v>74</v>
+        <v>512</v>
       </c>
       <c r="B69" t="s" s="1">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C69" t="s" s="1">
         <v>271</v>
@@ -3366,32 +3375,32 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="1">
-        <v>86</v>
+        <v>367</v>
       </c>
       <c r="B70" t="s" s="1">
-        <v>294</v>
+        <v>66</v>
       </c>
       <c r="C70" t="s" s="1">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="1">
-        <v>152</v>
+        <v>414</v>
       </c>
       <c r="B71" t="s" s="1">
-        <v>273</v>
+        <v>337</v>
       </c>
       <c r="C71" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="1">
-        <v>519</v>
+        <v>136</v>
       </c>
       <c r="B72" t="s" s="1">
-        <v>286</v>
+        <v>7</v>
       </c>
       <c r="C72" t="s" s="1">
         <v>271</v>
@@ -3399,21 +3408,21 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="1">
-        <v>248</v>
+        <v>82</v>
       </c>
       <c r="B73" t="s" s="1">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="C73" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="1">
-        <v>391</v>
+        <v>482</v>
       </c>
       <c r="B74" t="s" s="1">
-        <v>289</v>
+        <v>369</v>
       </c>
       <c r="C74" t="s" s="1">
         <v>271</v>
@@ -3421,32 +3430,32 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="1">
-        <v>387</v>
+        <v>204</v>
       </c>
       <c r="B75" t="s" s="1">
-        <v>273</v>
+        <v>45</v>
       </c>
       <c r="C75" t="s" s="1">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="1">
-        <v>217</v>
+        <v>86</v>
       </c>
       <c r="B76" t="s" s="1">
-        <v>280</v>
+        <v>69</v>
       </c>
       <c r="C76" t="s" s="1">
-        <v>5</v>
+        <v>270</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="1">
-        <v>144</v>
+        <v>366</v>
       </c>
       <c r="B77" t="s" s="1">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C77" t="s" s="1">
         <v>271</v>
@@ -3454,21 +3463,21 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="1">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="B78" t="s" s="1">
-        <v>101</v>
+        <v>274</v>
       </c>
       <c r="C78" t="s" s="1">
-        <v>5</v>
+        <v>268</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="1">
-        <v>433</v>
+        <v>99</v>
       </c>
       <c r="B79" t="s" s="1">
-        <v>273</v>
+        <v>27</v>
       </c>
       <c r="C79" t="s" s="1">
         <v>5</v>
@@ -3476,10 +3485,10 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="1">
-        <v>141</v>
+        <v>223</v>
       </c>
       <c r="B80" t="s" s="1">
-        <v>38</v>
+        <v>267</v>
       </c>
       <c r="C80" t="s" s="1">
         <v>270</v>
@@ -3487,32 +3496,32 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="1">
-        <v>153</v>
+        <v>306</v>
       </c>
       <c r="B81" t="s" s="1">
-        <v>520</v>
+        <v>297</v>
       </c>
       <c r="C81" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s" s="1">
-        <v>213</v>
+        <v>100</v>
       </c>
       <c r="B82" t="s" s="1">
-        <v>275</v>
+        <v>34</v>
       </c>
       <c r="C82" t="s" s="1">
-        <v>5</v>
+        <v>270</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s" s="1">
-        <v>500</v>
+        <v>240</v>
       </c>
       <c r="B83" t="s" s="1">
-        <v>289</v>
+        <v>23</v>
       </c>
       <c r="C83" t="s" s="1">
         <v>271</v>
@@ -3520,21 +3529,21 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="1">
-        <v>238</v>
+        <v>459</v>
       </c>
       <c r="B84" t="s" s="1">
         <v>286</v>
       </c>
       <c r="C84" t="s" s="1">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s" s="1">
-        <v>367</v>
+        <v>396</v>
       </c>
       <c r="B85" t="s" s="1">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C85" t="s" s="1">
         <v>271</v>
@@ -3542,21 +3551,21 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="1">
-        <v>193</v>
+        <v>112</v>
       </c>
       <c r="B86" t="s" s="1">
-        <v>324</v>
+        <v>301</v>
       </c>
       <c r="C86" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s" s="1">
-        <v>396</v>
+        <v>103</v>
       </c>
       <c r="B87" t="s" s="1">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C87" t="s" s="1">
         <v>271</v>
@@ -3564,10 +3573,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="1">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="B88" t="s" s="1">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C88" t="s" s="1">
         <v>271</v>
@@ -3575,10 +3584,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="1">
-        <v>233</v>
+        <v>190</v>
       </c>
       <c r="B89" t="s" s="1">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="C89" t="s" s="1">
         <v>271</v>
@@ -3586,54 +3595,54 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="1">
-        <v>154</v>
+        <v>354</v>
       </c>
       <c r="B90" t="s" s="1">
-        <v>66</v>
+        <v>286</v>
       </c>
       <c r="C90" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s" s="1">
-        <v>150</v>
+        <v>214</v>
       </c>
       <c r="B91" t="s" s="1">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C91" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s" s="1">
-        <v>138</v>
+        <v>303</v>
       </c>
       <c r="B92" t="s" s="1">
-        <v>390</v>
+        <v>289</v>
       </c>
       <c r="C92" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s" s="1">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="B93" t="s" s="1">
-        <v>279</v>
+        <v>84</v>
       </c>
       <c r="C93" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s" s="1">
-        <v>440</v>
+        <v>314</v>
       </c>
       <c r="B94" t="s" s="1">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="C94" t="s" s="1">
         <v>271</v>
@@ -3641,10 +3650,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s" s="1">
-        <v>162</v>
+        <v>523</v>
       </c>
       <c r="B95" t="s" s="1">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="C95" t="s" s="1">
         <v>5</v>
@@ -3655,7 +3664,7 @@
         <v>237</v>
       </c>
       <c r="B96" t="s" s="1">
-        <v>283</v>
+        <v>66</v>
       </c>
       <c r="C96" t="s" s="1">
         <v>271</v>
@@ -3663,21 +3672,21 @@
     </row>
     <row r="97">
       <c r="A97" t="s" s="1">
-        <v>195</v>
+        <v>447</v>
       </c>
       <c r="B97" t="s" s="1">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="C97" t="s" s="1">
-        <v>270</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s" s="1">
-        <v>264</v>
+        <v>332</v>
       </c>
       <c r="B98" t="s" s="1">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C98" t="s" s="1">
         <v>271</v>
@@ -3685,32 +3694,32 @@
     </row>
     <row r="99">
       <c r="A99" t="s" s="1">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="B99" t="s" s="1">
-        <v>276</v>
+        <v>34</v>
       </c>
       <c r="C99" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s" s="1">
-        <v>99</v>
+        <v>503</v>
       </c>
       <c r="B100" t="s" s="1">
-        <v>27</v>
+        <v>460</v>
       </c>
       <c r="C100" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s" s="1">
-        <v>24</v>
+        <v>442</v>
       </c>
       <c r="B101" t="s" s="1">
-        <v>66</v>
+        <v>287</v>
       </c>
       <c r="C101" t="s" s="1">
         <v>271</v>
@@ -3718,21 +3727,21 @@
     </row>
     <row r="102">
       <c r="A102" t="s" s="1">
-        <v>409</v>
+        <v>218</v>
       </c>
       <c r="B102" t="s" s="1">
-        <v>34</v>
+        <v>301</v>
       </c>
       <c r="C102" t="s" s="1">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s" s="1">
-        <v>142</v>
+        <v>407</v>
       </c>
       <c r="B103" t="s" s="1">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="C103" t="s" s="1">
         <v>271</v>
@@ -3740,10 +3749,10 @@
     </row>
     <row r="104">
       <c r="A104" t="s" s="1">
-        <v>214</v>
+        <v>397</v>
       </c>
       <c r="B104" t="s" s="1">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="C104" t="s" s="1">
         <v>271</v>
@@ -3751,10 +3760,10 @@
     </row>
     <row r="105">
       <c r="A105" t="s" s="1">
-        <v>381</v>
+        <v>20</v>
       </c>
       <c r="B105" t="s" s="1">
-        <v>301</v>
+        <v>267</v>
       </c>
       <c r="C105" t="s" s="1">
         <v>271</v>
@@ -3762,10 +3771,10 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="1">
-        <v>521</v>
+        <v>152</v>
       </c>
       <c r="B106" t="s" s="1">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C106" t="s" s="1">
         <v>271</v>
@@ -3773,10 +3782,10 @@
     </row>
     <row r="107">
       <c r="A107" t="s" s="1">
-        <v>429</v>
+        <v>222</v>
       </c>
       <c r="B107" t="s" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C107" t="s" s="1">
         <v>271</v>
@@ -3784,65 +3793,65 @@
     </row>
     <row r="108">
       <c r="A108" t="s" s="1">
-        <v>265</v>
+        <v>230</v>
       </c>
       <c r="B108" t="s" s="1">
-        <v>89</v>
+        <v>301</v>
       </c>
       <c r="C108" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s" s="1">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="B109" t="s" s="1">
-        <v>281</v>
+        <v>13</v>
       </c>
       <c r="C109" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s" s="1">
-        <v>522</v>
+        <v>113</v>
       </c>
       <c r="B110" t="s" s="1">
-        <v>284</v>
+        <v>17</v>
       </c>
       <c r="C110" t="s" s="1">
-        <v>271</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s" s="1">
-        <v>523</v>
+        <v>194</v>
       </c>
       <c r="B111" t="s" s="1">
-        <v>289</v>
+        <v>373</v>
       </c>
       <c r="C111" t="s" s="1">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s" s="1">
-        <v>234</v>
+        <v>46</v>
       </c>
       <c r="B112" t="s" s="1">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C112" t="s" s="1">
-        <v>271</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s" s="1">
-        <v>338</v>
+        <v>450</v>
       </c>
       <c r="B113" t="s" s="1">
-        <v>289</v>
+        <v>84</v>
       </c>
       <c r="C113" t="s" s="1">
         <v>271</v>
@@ -3850,87 +3859,87 @@
     </row>
     <row r="114">
       <c r="A114" t="s" s="1">
-        <v>113</v>
+        <v>317</v>
       </c>
       <c r="B114" t="s" s="1">
-        <v>524</v>
+        <v>273</v>
       </c>
       <c r="C114" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s" s="1">
-        <v>187</v>
+        <v>156</v>
       </c>
       <c r="B115" t="s" s="1">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="C115" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s" s="1">
-        <v>326</v>
+        <v>511</v>
       </c>
       <c r="B116" t="s" s="1">
-        <v>276</v>
+        <v>316</v>
       </c>
       <c r="C116" t="s" s="1">
-        <v>5</v>
+        <v>268</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s" s="1">
-        <v>31</v>
+        <v>177</v>
       </c>
       <c r="B117" t="s" s="1">
-        <v>69</v>
+        <v>527</v>
       </c>
       <c r="C117" t="s" s="1">
-        <v>268</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s" s="1">
-        <v>44</v>
+        <v>236</v>
       </c>
       <c r="B118" t="s" s="1">
-        <v>525</v>
+        <v>341</v>
       </c>
       <c r="C118" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s" s="1">
-        <v>87</v>
+        <v>217</v>
       </c>
       <c r="B119" t="s" s="1">
-        <v>79</v>
+        <v>280</v>
       </c>
       <c r="C119" t="s" s="1">
-        <v>271</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s" s="1">
-        <v>428</v>
+        <v>448</v>
       </c>
       <c r="B120" t="s" s="1">
-        <v>15</v>
+        <v>301</v>
       </c>
       <c r="C120" t="s" s="1">
-        <v>5</v>
+        <v>268</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s" s="1">
-        <v>82</v>
+        <v>468</v>
       </c>
       <c r="B121" t="s" s="1">
-        <v>27</v>
+        <v>337</v>
       </c>
       <c r="C121" t="s" s="1">
         <v>271</v>
@@ -3938,35 +3947,1245 @@
     </row>
     <row r="122">
       <c r="A122" t="s" s="1">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="B122" t="s" s="1">
-        <v>269</v>
+        <v>45</v>
       </c>
       <c r="C122" t="s" s="1">
-        <v>5</v>
+        <v>271</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s" s="1">
-        <v>262</v>
+        <v>330</v>
       </c>
       <c r="B123" t="s" s="1">
-        <v>267</v>
+        <v>4</v>
       </c>
       <c r="C123" t="s" s="1">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s" s="1">
-        <v>447</v>
+        <v>105</v>
       </c>
       <c r="B124" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C124" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s" s="1">
+        <v>211</v>
+      </c>
+      <c r="B125" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C125" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s" s="1">
+        <v>391</v>
+      </c>
+      <c r="B126" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C126" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s" s="1">
+        <v>80</v>
+      </c>
+      <c r="B127" t="s" s="1">
+        <v>276</v>
+      </c>
+      <c r="C127" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s" s="1">
+        <v>394</v>
+      </c>
+      <c r="B128" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C128" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s" s="1">
+        <v>415</v>
+      </c>
+      <c r="B129" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C129" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s" s="1">
+        <v>180</v>
+      </c>
+      <c r="B130" t="s" s="1">
+        <v>301</v>
+      </c>
+      <c r="C130" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s" s="1">
+        <v>216</v>
+      </c>
+      <c r="B131" t="s" s="1">
+        <v>273</v>
+      </c>
+      <c r="C131" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s" s="1">
+        <v>487</v>
+      </c>
+      <c r="B132" t="s" s="1">
+        <v>13</v>
+      </c>
+      <c r="C132" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s" s="1">
+        <v>471</v>
+      </c>
+      <c r="B133" t="s" s="1">
+        <v>45</v>
+      </c>
+      <c r="C133" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="B134" t="s" s="1">
+        <v>460</v>
+      </c>
+      <c r="C134" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s" s="1">
+        <v>135</v>
+      </c>
+      <c r="B135" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C135" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s" s="1">
+        <v>452</v>
+      </c>
+      <c r="B136" t="s" s="1">
+        <v>111</v>
+      </c>
+      <c r="C136" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s" s="1">
+        <v>189</v>
+      </c>
+      <c r="B137" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C137" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s" s="1">
+        <v>477</v>
+      </c>
+      <c r="B138" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C138" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s" s="1">
+        <v>418</v>
+      </c>
+      <c r="B139" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C139" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s" s="1">
+        <v>479</v>
+      </c>
+      <c r="B140" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="C140" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s" s="1">
+        <v>420</v>
+      </c>
+      <c r="B141" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="C141" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s" s="1">
+        <v>393</v>
+      </c>
+      <c r="B142" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C142" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s" s="1">
+        <v>387</v>
+      </c>
+      <c r="B143" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="C143" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s" s="1">
+        <v>380</v>
+      </c>
+      <c r="B144" t="s" s="1">
+        <v>38</v>
+      </c>
+      <c r="C144" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s" s="1">
+        <v>172</v>
+      </c>
+      <c r="B145" t="s" s="1">
+        <v>38</v>
+      </c>
+      <c r="C145" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s" s="1">
+        <v>133</v>
+      </c>
+      <c r="B146" t="s" s="1">
+        <v>116</v>
+      </c>
+      <c r="C146" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s" s="1">
+        <v>416</v>
+      </c>
+      <c r="B147" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C147" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s" s="1">
+        <v>221</v>
+      </c>
+      <c r="B148" t="s" s="1">
+        <v>111</v>
+      </c>
+      <c r="C148" t="s" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s" s="1">
+        <v>312</v>
+      </c>
+      <c r="B149" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C149" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s" s="1">
+        <v>336</v>
+      </c>
+      <c r="B150" t="s" s="1">
+        <v>337</v>
+      </c>
+      <c r="C150" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s" s="1">
+        <v>151</v>
+      </c>
+      <c r="B151" t="s" s="1">
+        <v>116</v>
+      </c>
+      <c r="C151" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s" s="1">
+        <v>363</v>
+      </c>
+      <c r="B152" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C152" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s" s="1">
+        <v>323</v>
+      </c>
+      <c r="B153" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C153" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s" s="1">
+        <v>368</v>
+      </c>
+      <c r="B154" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C154" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s" s="1">
+        <v>115</v>
+      </c>
+      <c r="B155" t="s" s="1">
+        <v>111</v>
+      </c>
+      <c r="C155" t="s" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s" s="1">
+        <v>123</v>
+      </c>
+      <c r="B156" t="s" s="1">
+        <v>38</v>
+      </c>
+      <c r="C156" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s" s="1">
+        <v>24</v>
+      </c>
+      <c r="B157" t="s" s="1">
+        <v>45</v>
+      </c>
+      <c r="C157" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s" s="1">
+        <v>454</v>
+      </c>
+      <c r="B158" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="C158" t="s" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s" s="1">
+        <v>417</v>
+      </c>
+      <c r="B159" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C159" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s" s="1">
+        <v>117</v>
+      </c>
+      <c r="B160" t="s" s="1">
+        <v>277</v>
+      </c>
+      <c r="C160" t="s" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s" s="1">
+        <v>319</v>
+      </c>
+      <c r="B161" t="s" s="1">
+        <v>66</v>
+      </c>
+      <c r="C161" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="B162" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="C162" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s" s="1">
+        <v>402</v>
+      </c>
+      <c r="B163" t="s" s="1">
+        <v>69</v>
+      </c>
+      <c r="C163" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s" s="1">
+        <v>167</v>
+      </c>
+      <c r="B164" t="s" s="1">
+        <v>352</v>
+      </c>
+      <c r="C164" t="s" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s" s="1">
+        <v>59</v>
+      </c>
+      <c r="B165" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C165" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s" s="1">
+        <v>400</v>
+      </c>
+      <c r="B166" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C166" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s" s="1">
+        <v>439</v>
+      </c>
+      <c r="B167" t="s" s="1">
+        <v>7</v>
+      </c>
+      <c r="C167" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s" s="1">
+        <v>318</v>
+      </c>
+      <c r="B168" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="C168" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s" s="1">
+        <v>506</v>
+      </c>
+      <c r="B169" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C169" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s" s="1">
+        <v>343</v>
+      </c>
+      <c r="B170" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C170" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s" s="1">
+        <v>246</v>
+      </c>
+      <c r="B171" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="C171" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s" s="1">
+        <v>361</v>
+      </c>
+      <c r="B172" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C172" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s" s="1">
+        <v>309</v>
+      </c>
+      <c r="B173" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="C173" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s" s="1">
+        <v>184</v>
+      </c>
+      <c r="B174" t="s" s="1">
+        <v>301</v>
+      </c>
+      <c r="C174" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="B175" t="s" s="1">
+        <v>283</v>
+      </c>
+      <c r="C175" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="B176" t="s" s="1">
+        <v>84</v>
+      </c>
+      <c r="C176" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s" s="1">
+        <v>434</v>
+      </c>
+      <c r="B177" t="s" s="1">
+        <v>84</v>
+      </c>
+      <c r="C177" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s" s="1">
+        <v>470</v>
+      </c>
+      <c r="B178" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C178" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s" s="1">
+        <v>358</v>
+      </c>
+      <c r="B179" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C179" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s" s="1">
+        <v>212</v>
+      </c>
+      <c r="B180" t="s" s="1">
         <v>23</v>
       </c>
-      <c r="C124" t="s" s="1">
+      <c r="C180" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s" s="1">
+        <v>300</v>
+      </c>
+      <c r="B181" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C181" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s" s="1">
+        <v>342</v>
+      </c>
+      <c r="B182" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C182" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s" s="1">
+        <v>430</v>
+      </c>
+      <c r="B183" t="s" s="1">
+        <v>460</v>
+      </c>
+      <c r="C183" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s" s="1">
+        <v>132</v>
+      </c>
+      <c r="B184" t="s" s="1">
+        <v>45</v>
+      </c>
+      <c r="C184" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s" s="1">
+        <v>321</v>
+      </c>
+      <c r="B185" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C185" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s" s="1">
+        <v>486</v>
+      </c>
+      <c r="B186" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C186" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s" s="1">
+        <v>164</v>
+      </c>
+      <c r="B187" t="s" s="1">
+        <v>276</v>
+      </c>
+      <c r="C187" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="B188" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="C188" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="B189" t="s" s="1">
+        <v>66</v>
+      </c>
+      <c r="C189" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s" s="1">
+        <v>514</v>
+      </c>
+      <c r="B190" t="s" s="1">
+        <v>45</v>
+      </c>
+      <c r="C190" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s" s="1">
+        <v>409</v>
+      </c>
+      <c r="B191" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C191" t="s" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s" s="1">
+        <v>315</v>
+      </c>
+      <c r="B192" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C192" t="s" s="1">
         <v>5</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s" s="1">
+        <v>509</v>
+      </c>
+      <c r="B193" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="C193" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s" s="1">
+        <v>508</v>
+      </c>
+      <c r="B194" t="s" s="1">
+        <v>499</v>
+      </c>
+      <c r="C194" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s" s="1">
+        <v>75</v>
+      </c>
+      <c r="B195" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C195" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s" s="1">
+        <v>185</v>
+      </c>
+      <c r="B196" t="s" s="1">
+        <v>273</v>
+      </c>
+      <c r="C196" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s" s="1">
+        <v>160</v>
+      </c>
+      <c r="B197" t="s" s="1">
+        <v>313</v>
+      </c>
+      <c r="C197" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s" s="1">
+        <v>171</v>
+      </c>
+      <c r="B198" t="s" s="1">
+        <v>84</v>
+      </c>
+      <c r="C198" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s" s="1">
+        <v>320</v>
+      </c>
+      <c r="B199" t="s" s="1">
+        <v>107</v>
+      </c>
+      <c r="C199" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s" s="1">
+        <v>500</v>
+      </c>
+      <c r="B200" t="s" s="1">
+        <v>66</v>
+      </c>
+      <c r="C200" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s" s="1">
+        <v>213</v>
+      </c>
+      <c r="B201" t="s" s="1">
+        <v>66</v>
+      </c>
+      <c r="C201" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s" s="1">
+        <v>51</v>
+      </c>
+      <c r="B202" t="s" s="1">
+        <v>45</v>
+      </c>
+      <c r="C202" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s" s="1">
+        <v>106</v>
+      </c>
+      <c r="B203" t="s" s="1">
+        <v>52</v>
+      </c>
+      <c r="C203" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s" s="1">
+        <v>193</v>
+      </c>
+      <c r="B204" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="C204" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B205" t="s" s="1">
+        <v>329</v>
+      </c>
+      <c r="C205" t="s" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s" s="1">
+        <v>362</v>
+      </c>
+      <c r="B206" t="s" s="1">
+        <v>276</v>
+      </c>
+      <c r="C206" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s" s="1">
+        <v>305</v>
+      </c>
+      <c r="B207" t="s" s="1">
+        <v>276</v>
+      </c>
+      <c r="C207" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s" s="1">
+        <v>88</v>
+      </c>
+      <c r="B208" t="s" s="1">
+        <v>11</v>
+      </c>
+      <c r="C208" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s" s="1">
+        <v>388</v>
+      </c>
+      <c r="B209" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C209" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s" s="1">
+        <v>345</v>
+      </c>
+      <c r="B210" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C210" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s" s="1">
+        <v>227</v>
+      </c>
+      <c r="B211" t="s" s="1">
+        <v>273</v>
+      </c>
+      <c r="C211" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s" s="1">
+        <v>234</v>
+      </c>
+      <c r="B212" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C212" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B213" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C213" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s" s="1">
+        <v>250</v>
+      </c>
+      <c r="B214" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C214" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s" s="1">
+        <v>235</v>
+      </c>
+      <c r="B215" t="s" s="1">
+        <v>79</v>
+      </c>
+      <c r="C215" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="B216" t="s" s="1">
+        <v>528</v>
+      </c>
+      <c r="C216" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s" s="1">
+        <v>302</v>
+      </c>
+      <c r="B217" t="s" s="1">
+        <v>66</v>
+      </c>
+      <c r="C217" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s" s="1">
+        <v>469</v>
+      </c>
+      <c r="B218" t="s" s="1">
+        <v>273</v>
+      </c>
+      <c r="C218" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s" s="1">
+        <v>325</v>
+      </c>
+      <c r="B219" t="s" s="1">
+        <v>84</v>
+      </c>
+      <c r="C219" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s" s="1">
+        <v>493</v>
+      </c>
+      <c r="B220" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C220" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s" s="1">
+        <v>224</v>
+      </c>
+      <c r="B221" t="s" s="1">
+        <v>276</v>
+      </c>
+      <c r="C221" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s" s="1">
+        <v>239</v>
+      </c>
+      <c r="B222" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="C222" t="s" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s" s="1">
+        <v>145</v>
+      </c>
+      <c r="B223" t="s" s="1">
+        <v>276</v>
+      </c>
+      <c r="C223" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s" s="1">
+        <v>119</v>
+      </c>
+      <c r="B224" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="C224" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s" s="1">
+        <v>195</v>
+      </c>
+      <c r="B225" t="s" s="1">
+        <v>63</v>
+      </c>
+      <c r="C225" t="s" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s" s="1">
+        <v>55</v>
+      </c>
+      <c r="B226" t="s" s="1">
+        <v>23</v>
+      </c>
+      <c r="C226" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s" s="1">
+        <v>378</v>
+      </c>
+      <c r="B227" t="s" s="1">
+        <v>301</v>
+      </c>
+      <c r="C227" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s" s="1">
+        <v>412</v>
+      </c>
+      <c r="B228" t="s" s="1">
+        <v>301</v>
+      </c>
+      <c r="C228" t="s" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s" s="1">
+        <v>433</v>
+      </c>
+      <c r="B229" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C229" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s" s="1">
+        <v>231</v>
+      </c>
+      <c r="B230" t="s" s="1">
+        <v>285</v>
+      </c>
+      <c r="C230" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s" s="1">
+        <v>56</v>
+      </c>
+      <c r="B231" t="s" s="1">
+        <v>11</v>
+      </c>
+      <c r="C231" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s" s="1">
+        <v>110</v>
+      </c>
+      <c r="B232" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="C232" t="s" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s" s="1">
+        <v>389</v>
+      </c>
+      <c r="B233" t="s" s="1">
+        <v>23</v>
+      </c>
+      <c r="C233" t="s" s="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s" s="1">
+        <v>71</v>
+      </c>
+      <c r="B234" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C234" t="s" s="1">
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>